<commit_message>
add 20200504 BIM data
</commit_message>
<xml_diff>
--- a/data/tle/Breakage_report.xlsx
+++ b/data/tle/Breakage_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/bsrte/data/tle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AD0C3C-6F1D-844E-BB66-B890491159A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F219DBC-636B-A442-ACC2-3CF1081EC823}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1040" windowWidth="27640" windowHeight="16540" xr2:uid="{C71E0CC0-8BE9-D747-9ADD-2DAB0B5FDB15}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>nursery</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>breakage</t>
+  </si>
+  <si>
+    <t>3cm branch has died</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288B9E20-A8A6-5547-A0BD-CB92B37C5971}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,6 +483,26 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>147</v>
+      </c>
+      <c r="C4">
+        <v>96</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>20200504</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>